<commit_message>
Added new test files
To test my new mapping tools have added some more complex files to test
</commit_message>
<xml_diff>
--- a/resources/b1.xlsx
+++ b/resources/b1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="1">
   <si>
     <t>INSERT</t>
   </si>
@@ -358,15 +358,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2</v>
       </c>
@@ -375,191 +373,118 @@
         <v>2</v>
       </c>
       <c r="C1">
-        <f t="shared" ref="C1:G1" si="0">B1</f>
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
+        <f t="shared" ref="C1:F1" si="0">B1</f>
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <f>C1</f>
+        <v>2</v>
       </c>
       <c r="E1">
-        <f>C1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A4</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>B4</f>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>C4</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f>D4</f>
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <f>E4</f>
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f>F4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <f>A1</f>
         <v>2</v>
       </c>
-      <c r="B2">
-        <f t="shared" ref="B2:G7" si="1">B1</f>
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <f t="shared" si="1"/>
+      <c r="B4">
+        <f>B1</f>
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>C1</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f>D1</f>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>E1</f>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f>F1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ref="A3:A7" si="2">A2</f>
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>A3</f>
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <f>B3</f>
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <f>C3</f>
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>E3</f>
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <f>F3</f>
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <f>G3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>2</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B5" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C5" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D5" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E5" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F5" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>